<commit_message>
add test runner to pom run tests
</commit_message>
<xml_diff>
--- a/reports/Appium_Report.xlsx
+++ b/reports/Appium_Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="105">
   <si>
     <t>Category</t>
   </si>
@@ -49,19 +49,19 @@
     <t>Start Time</t>
   </si>
   <si>
-    <t>2020-02-05T16:02:34 IST</t>
+    <t>Feb 06, 2020 07:18:09 PM</t>
   </si>
   <si>
     <t>End Time</t>
   </si>
   <si>
-    <t>2020-02-05T16:09:00 IST</t>
+    <t>Feb 06, 2020 07:24:38 PM</t>
   </si>
   <si>
     <t>Duration</t>
   </si>
   <si>
-    <t>385229 ms</t>
+    <t>389460 ms</t>
   </si>
   <si>
     <t>TestCase Name</t>
@@ -82,13 +82,13 @@
     <t>Error message was not displayed correctly expected [Authentication failed!] but found [Authentication failed.]</t>
   </si>
   <si>
-    <t>2020-02-05T16:02:42 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:02:53 IST</t>
-  </si>
-  <si>
-    <t>11265 ms</t>
+    <t>Feb 06, 2020 07:18:16 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:18:28 PM</t>
+  </si>
+  <si>
+    <t>12146 ms</t>
   </si>
   <si>
     <t>com.ios.web.test.WebBrowserTest.validLoginTest</t>
@@ -100,25 +100,25 @@
     <t/>
   </si>
   <si>
-    <t>2020-02-05T16:03:00 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:04:12 IST</t>
-  </si>
-  <si>
-    <t>71621 ms</t>
+    <t>Feb 06, 2020 07:18:35 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:19:45 PM</t>
+  </si>
+  <si>
+    <t>69453 ms</t>
   </si>
   <si>
     <t>com.ios.app.test.UIKitCatalogTest.enterText</t>
   </si>
   <si>
-    <t>2020-02-05T16:04:19 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:04:24 IST</t>
-  </si>
-  <si>
-    <t>5071 ms</t>
+    <t>Feb 06, 2020 07:19:52 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:19:57 PM</t>
+  </si>
+  <si>
+    <t>4964 ms</t>
   </si>
   <si>
     <t>com.ios.app.test.UIKitCatalogTest.getStepperCountTest</t>
@@ -127,109 +127,109 @@
     <t>CUSTOM Stepper count is not matichg expected [6] but found [5]</t>
   </si>
   <si>
-    <t>2020-02-05T16:04:31 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:04:51 IST</t>
-  </si>
-  <si>
-    <t>20072 ms</t>
+    <t>Feb 06, 2020 07:20:04 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:20:24 PM</t>
+  </si>
+  <si>
+    <t>20141 ms</t>
   </si>
   <si>
     <t>com.ios.app.test.UIKitCatalogTest.pickerWheelTest</t>
   </si>
   <si>
-    <t>2020-02-05T16:04:58 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:05:03 IST</t>
-  </si>
-  <si>
-    <t>4521 ms</t>
+    <t>Feb 06, 2020 07:20:31 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:20:36 PM</t>
+  </si>
+  <si>
+    <t>4519 ms</t>
   </si>
   <si>
     <t>com.ios.app.test.UIKitCatalogTest.scrollTest</t>
   </si>
   <si>
-    <t>2020-02-05T16:05:10 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:05:11 IST</t>
-  </si>
-  <si>
-    <t>1050 ms</t>
+    <t>Feb 06, 2020 07:20:43 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:20:44 PM</t>
+  </si>
+  <si>
+    <t>1088 ms</t>
   </si>
   <si>
     <t>com.ios.app.test.UIKitCatalogTest.sliderTest</t>
   </si>
   <si>
-    <t>2020-02-05T16:05:18 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:05:28 IST</t>
-  </si>
-  <si>
-    <t>10360 ms</t>
+    <t>Feb 06, 2020 07:20:51 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:21:01 PM</t>
+  </si>
+  <si>
+    <t>10529 ms</t>
   </si>
   <si>
     <t>com.ios.app.test.UIKitCatalogTest.tapTest</t>
   </si>
   <si>
-    <t>2020-02-05T16:05:34 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:05:39 IST</t>
-  </si>
-  <si>
-    <t>4857 ms</t>
+    <t>Feb 06, 2020 07:21:08 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:21:13 PM</t>
+  </si>
+  <si>
+    <t>4752 ms</t>
   </si>
   <si>
     <t>com.ios.app.test.UIKitCatalogTest.zoomOperations</t>
   </si>
   <si>
-    <t>2020-02-05T16:05:46 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:05:52 IST</t>
-  </si>
-  <si>
-    <t>6513 ms</t>
+    <t>Feb 06, 2020 07:21:20 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:21:26 PM</t>
+  </si>
+  <si>
+    <t>6519 ms</t>
   </si>
   <si>
     <t>com.android.app.test.GenralStoreTest.addProductToCart</t>
   </si>
   <si>
-    <t>2020-02-05T16:02:43 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:03:19 IST</t>
-  </si>
-  <si>
-    <t>35797 ms</t>
+    <t>Feb 06, 2020 07:18:17 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:18:55 PM</t>
+  </si>
+  <si>
+    <t>37385 ms</t>
   </si>
   <si>
     <t>com.android.app.test.GenralStoreTest.fillShoppingForm</t>
   </si>
   <si>
-    <t>2020-02-05T16:03:27 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:03:35 IST</t>
-  </si>
-  <si>
-    <t>7795 ms</t>
+    <t>Feb 06, 2020 07:19:03 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:19:11 PM</t>
+  </si>
+  <si>
+    <t>7936 ms</t>
   </si>
   <si>
     <t>com.android.app.test.GenralStoreTest.mobileGesturesOnCart</t>
   </si>
   <si>
-    <t>2020-02-05T16:03:44 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:04:23 IST</t>
-  </si>
-  <si>
-    <t>38877 ms</t>
+    <t>Feb 06, 2020 07:19:18 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:19:58 PM</t>
+  </si>
+  <si>
+    <t>39500 ms</t>
   </si>
   <si>
     <t>com.android.app.test.GenralStoreTest.shoppingFormErrorValidation</t>
@@ -238,100 +238,97 @@
     <t>Valid Error message was not displayed expected [Please enter your user name] but found [Please enter your name]</t>
   </si>
   <si>
-    <t>2020-02-05T16:04:52 IST</t>
-  </si>
-  <si>
-    <t>20762 ms</t>
+    <t>Feb 06, 2020 07:20:06 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:20:27 PM</t>
+  </si>
+  <si>
+    <t>21039 ms</t>
   </si>
   <si>
     <t>com.android.app.test.GenralStoreTest.testSwitchingFromNativeToWebAndBack</t>
   </si>
   <si>
-    <t>2020-02-05T16:05:01 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:05:54 IST</t>
-  </si>
-  <si>
-    <t>53674 ms</t>
+    <t>Feb 06, 2020 07:21:31 PM</t>
+  </si>
+  <si>
+    <t>54810 ms</t>
   </si>
   <si>
     <t>com.android.app.test.GenralStoreTest.validateSumOfProductsInCart</t>
   </si>
   <si>
-    <t>2020-02-05T16:06:01 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:06:58 IST</t>
-  </si>
-  <si>
-    <t>56673 ms</t>
+    <t>Feb 06, 2020 07:21:38 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:22:35 PM</t>
+  </si>
+  <si>
+    <t>57156 ms</t>
   </si>
   <si>
     <t>com.android.installed.app.test.CalculatorAppTest.testCalculator</t>
   </si>
   <si>
-    <t>2020-02-05T16:07:04 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:07:12 IST</t>
-  </si>
-  <si>
-    <t>7794 ms</t>
+    <t>Feb 06, 2020 07:22:41 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:22:48 PM</t>
+  </si>
+  <si>
+    <t>6747 ms</t>
   </si>
   <si>
     <t>Result did not match expected [10] but found [100]</t>
   </si>
   <si>
-    <t>2020-02-05T16:07:18 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:07:23 IST</t>
-  </si>
-  <si>
-    <t>4920 ms</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:07:30 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:07:37 IST</t>
-  </si>
-  <si>
-    <t>7531 ms</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:07:44 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:07:50 IST</t>
-  </si>
-  <si>
-    <t>5705 ms</t>
+    <t>Feb 06, 2020 07:22:55 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:23:00 PM</t>
+  </si>
+  <si>
+    <t>4876 ms</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:23:06 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:23:13 PM</t>
+  </si>
+  <si>
+    <t>6488 ms</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:23:19 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:23:25 PM</t>
+  </si>
+  <si>
+    <t>5904 ms</t>
   </si>
   <si>
     <t>com.android.web.test.WebBrowserTest.invalidLoginTest</t>
   </si>
   <si>
-    <t>2020-02-05T16:08:05 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:08:14 IST</t>
-  </si>
-  <si>
-    <t>9225 ms</t>
+    <t>Feb 06, 2020 07:23:43 PM</t>
+  </si>
+  <si>
+    <t>Feb 06, 2020 07:23:51 PM</t>
+  </si>
+  <si>
+    <t>8600 ms</t>
   </si>
   <si>
     <t>com.android.web.test.WebBrowserTest.validLoginTest</t>
   </si>
   <si>
-    <t>2020-02-05T16:08:30 IST</t>
-  </si>
-  <si>
-    <t>2020-02-05T16:08:59 IST</t>
-  </si>
-  <si>
-    <t>28828 ms</t>
+    <t>Feb 06, 2020 07:24:07 PM</t>
+  </si>
+  <si>
+    <t>30701 ms</t>
   </si>
 </sst>
 </file>
@@ -348,11 +345,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Comic Sans MS"/>
+      <name val="Times New Roman"/>
       <sz val="12.0"/>
     </font>
     <font>
-      <name val="Comic Sans MS"/>
+      <name val="Times New Roman"/>
       <sz val="14.0"/>
       <b val="true"/>
     </font>
@@ -676,8 +673,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.57421875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="26.578125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.28125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="22.4296875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -759,12 +756,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="53.87109375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="8.84765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="104.8046875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="26.578125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="26.578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="10.90234375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="46.0859375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="7.3046875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="89.39453125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="22.4296875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="22.4296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.15234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -981,12 +978,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="76.10546875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="8.84765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="107.671875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="26.578125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="26.578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="10.90234375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="65.85546875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="7.3046875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="92.7265625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="22.4296875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="22.4296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.15234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1080,18 +1077,18 @@
         <v>73</v>
       </c>
       <c r="D5" s="106" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="E5" s="107" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F5" s="108" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="109" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B6" s="110" t="s">
         <v>26</v>
@@ -1100,7 +1097,7 @@
         <v>27</v>
       </c>
       <c r="D6" s="112" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E6" s="113" t="s">
         <v>78</v>
@@ -1243,10 +1240,10 @@
         <v>103</v>
       </c>
       <c r="E13" s="155" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="156" t="s">
         <v>104</v>
-      </c>
-      <c r="F13" s="156" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>